<commit_message>
Added unit info button logic
</commit_message>
<xml_diff>
--- a/Project Specs/AndroidCombatGameSprints.xlsx
+++ b/Project Specs/AndroidCombatGameSprints.xlsx
@@ -525,7 +525,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
   <si>
     <t>Backlog ID</t>
   </si>
@@ -873,6 +873,12 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Vison method for player</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -2657,7 +2663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3003,28 +3009,21 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="62" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="65" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="36" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="66" borderId="66" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="39" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="69" fillId="72" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="61" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="18" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="51" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3050,28 +3049,29 @@
     <xf numFmtId="0" fontId="79" fillId="32" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="65" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="61" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="69" fillId="72" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="5" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="20" fillId="18" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="66" borderId="66" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="62" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="62" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="36" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="39" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="51" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3079,22 +3079,31 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="66" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="62" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="66" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="80" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3137,7 +3146,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3283,11 +3291,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="51859456"/>
-        <c:axId val="88111296"/>
+        <c:axId val="49337856"/>
+        <c:axId val="110938944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51859456"/>
+        <c:axId val="49337856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3306,14 +3314,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88111296"/>
+        <c:crossAx val="110938944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3321,7 +3328,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88111296"/>
+        <c:axId val="110938944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3344,7 +3351,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
@@ -3366,7 +3372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51859456"/>
+        <c:crossAx val="49337856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3413,7 +3419,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3559,11 +3564,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54059008"/>
-        <c:axId val="53160192"/>
+        <c:axId val="49745920"/>
+        <c:axId val="110940096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54059008"/>
+        <c:axId val="49745920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,14 +3587,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53160192"/>
+        <c:crossAx val="110940096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3597,7 +3601,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53160192"/>
+        <c:axId val="110940096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3620,7 +3624,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
@@ -3642,7 +3645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54059008"/>
+        <c:crossAx val="49745920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3682,7 +3685,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3828,11 +3830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="56202752"/>
-        <c:axId val="53718976"/>
+        <c:axId val="50757632"/>
+        <c:axId val="110941824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56202752"/>
+        <c:axId val="50757632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3851,14 +3853,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53718976"/>
+        <c:crossAx val="110941824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3866,7 +3867,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53718976"/>
+        <c:axId val="110941824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3889,7 +3890,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
@@ -3911,7 +3911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56202752"/>
+        <c:crossAx val="50757632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4095,11 +4095,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="55823872"/>
-        <c:axId val="53720704"/>
+        <c:axId val="49232384"/>
+        <c:axId val="110942976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55823872"/>
+        <c:axId val="49232384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4124,7 +4124,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53720704"/>
+        <c:crossAx val="110942976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4132,7 +4132,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53720704"/>
+        <c:axId val="110942976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4175,7 +4175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55823872"/>
+        <c:crossAx val="49232384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7777,449 +7777,449 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="143" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
       <c r="D1" s="69">
         <v>1</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="139"/>
+      <c r="R1" s="139"/>
+      <c r="S1" s="139"/>
+      <c r="T1" s="139"/>
+      <c r="U1" s="139"/>
+      <c r="V1" s="139"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="139"/>
     </row>
     <row r="2" spans="1:24" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="139"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="139"/>
+      <c r="S2" s="139"/>
+      <c r="T2" s="139"/>
+      <c r="U2" s="139"/>
+      <c r="V2" s="139"/>
+      <c r="W2" s="139"/>
+      <c r="X2" s="139"/>
     </row>
     <row r="3" spans="1:24" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="128"/>
+      <c r="C3" s="146"/>
       <c r="D3" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="129" t="s">
+      <c r="E3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="129"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="129"/>
-      <c r="S3" s="129"/>
-      <c r="T3" s="129"/>
-      <c r="U3" s="129"/>
-      <c r="V3" s="129"/>
-      <c r="W3" s="129"/>
-      <c r="X3" s="129"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="141"/>
+      <c r="O3" s="141"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="141"/>
+      <c r="T3" s="141"/>
+      <c r="U3" s="141"/>
+      <c r="V3" s="141"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="141"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66">
         <v>1</v>
       </c>
-      <c r="B4" s="127">
+      <c r="B4" s="142">
         <v>20</v>
       </c>
-      <c r="C4" s="127"/>
+      <c r="C4" s="142"/>
       <c r="D4" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="124"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="139"/>
+      <c r="T4" s="139"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67">
         <v>2</v>
       </c>
-      <c r="B5" s="127">
+      <c r="B5" s="142">
         <v>20</v>
       </c>
-      <c r="C5" s="127"/>
+      <c r="C5" s="142"/>
       <c r="D5" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="139"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="139"/>
+      <c r="S5" s="139"/>
+      <c r="T5" s="139"/>
+      <c r="U5" s="139"/>
+      <c r="V5" s="139"/>
+      <c r="W5" s="139"/>
+      <c r="X5" s="139"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="67">
         <v>3</v>
       </c>
-      <c r="B6" s="124">
+      <c r="B6" s="139">
         <v>20</v>
       </c>
-      <c r="C6" s="124"/>
+      <c r="C6" s="139"/>
       <c r="D6" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="127"/>
-      <c r="U6" s="127"/>
-      <c r="V6" s="127"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="127"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
+      <c r="J6" s="142"/>
+      <c r="K6" s="142"/>
+      <c r="L6" s="142"/>
+      <c r="M6" s="142"/>
+      <c r="N6" s="142"/>
+      <c r="O6" s="142"/>
+      <c r="P6" s="142"/>
+      <c r="Q6" s="142"/>
+      <c r="R6" s="142"/>
+      <c r="S6" s="142"/>
+      <c r="T6" s="142"/>
+      <c r="U6" s="142"/>
+      <c r="V6" s="142"/>
+      <c r="W6" s="142"/>
+      <c r="X6" s="142"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="67">
         <v>4</v>
       </c>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
       <c r="D7" s="66"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
-      <c r="T7" s="127"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="127"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="127"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="142"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
+      <c r="V7" s="142"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="142"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="67">
         <v>5</v>
       </c>
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
       <c r="D8" s="67"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="127"/>
-      <c r="P8" s="127"/>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="127"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="127"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
+      <c r="H8" s="142"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="142"/>
+      <c r="N8" s="142"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="142"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="142"/>
+      <c r="S8" s="142"/>
+      <c r="T8" s="142"/>
+      <c r="U8" s="142"/>
+      <c r="V8" s="142"/>
+      <c r="W8" s="142"/>
+      <c r="X8" s="142"/>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="67">
         <v>6</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="124"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
       <c r="D9" s="67"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="124"/>
-      <c r="X9" s="124"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="139"/>
+      <c r="O9" s="139"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="139"/>
+      <c r="S9" s="139"/>
+      <c r="T9" s="139"/>
+      <c r="U9" s="139"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="139"/>
+      <c r="X9" s="139"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="67">
         <v>7</v>
       </c>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
       <c r="D10" s="67"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="124"/>
-      <c r="Q10" s="124"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="124"/>
-      <c r="T10" s="124"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="124"/>
-      <c r="W10" s="124"/>
-      <c r="X10" s="124"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="139"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="139"/>
+      <c r="M10" s="139"/>
+      <c r="N10" s="139"/>
+      <c r="O10" s="139"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="139"/>
+      <c r="R10" s="139"/>
+      <c r="S10" s="139"/>
+      <c r="T10" s="139"/>
+      <c r="U10" s="139"/>
+      <c r="V10" s="139"/>
+      <c r="W10" s="139"/>
+      <c r="X10" s="139"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67">
         <v>8</v>
       </c>
-      <c r="B11" s="124"/>
-      <c r="C11" s="124"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="67"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-      <c r="Q11" s="124"/>
-      <c r="R11" s="124"/>
-      <c r="S11" s="124"/>
-      <c r="T11" s="124"/>
-      <c r="U11" s="124"/>
-      <c r="V11" s="124"/>
-      <c r="W11" s="124"/>
-      <c r="X11" s="124"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="139"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="139"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="139"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="139"/>
+      <c r="N11" s="139"/>
+      <c r="O11" s="139"/>
+      <c r="P11" s="139"/>
+      <c r="Q11" s="139"/>
+      <c r="R11" s="139"/>
+      <c r="S11" s="139"/>
+      <c r="T11" s="139"/>
+      <c r="U11" s="139"/>
+      <c r="V11" s="139"/>
+      <c r="W11" s="139"/>
+      <c r="X11" s="139"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="67">
         <v>9</v>
       </c>
-      <c r="B12" s="124"/>
-      <c r="C12" s="124"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="67"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-      <c r="Q12" s="124"/>
-      <c r="R12" s="124"/>
-      <c r="S12" s="124"/>
-      <c r="T12" s="124"/>
-      <c r="U12" s="124"/>
-      <c r="V12" s="124"/>
-      <c r="W12" s="124"/>
-      <c r="X12" s="124"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="139"/>
+      <c r="N12" s="139"/>
+      <c r="O12" s="139"/>
+      <c r="P12" s="139"/>
+      <c r="Q12" s="139"/>
+      <c r="R12" s="139"/>
+      <c r="S12" s="139"/>
+      <c r="T12" s="139"/>
+      <c r="U12" s="139"/>
+      <c r="V12" s="139"/>
+      <c r="W12" s="139"/>
+      <c r="X12" s="139"/>
     </row>
     <row r="13" spans="1:24" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="67">
         <v>10</v>
       </c>
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
       <c r="D13" s="67"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-      <c r="Q13" s="124"/>
-      <c r="R13" s="124"/>
-      <c r="S13" s="124"/>
-      <c r="T13" s="124"/>
-      <c r="U13" s="124"/>
-      <c r="V13" s="124"/>
-      <c r="W13" s="124"/>
-      <c r="X13" s="124"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="139"/>
+      <c r="N13" s="139"/>
+      <c r="O13" s="139"/>
+      <c r="P13" s="139"/>
+      <c r="Q13" s="139"/>
+      <c r="R13" s="139"/>
+      <c r="S13" s="139"/>
+      <c r="T13" s="139"/>
+      <c r="U13" s="139"/>
+      <c r="V13" s="139"/>
+      <c r="W13" s="139"/>
+      <c r="X13" s="139"/>
     </row>
     <row r="14" spans="1:24" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="67"/>
-      <c r="B14" s="130">
+      <c r="B14" s="140">
         <f>SUM(B4:C13)</f>
         <v>60</v>
       </c>
-      <c r="C14" s="130"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="67"/>
-      <c r="E14" s="129" t="s">
+      <c r="E14" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="129"/>
+      <c r="F14" s="141"/>
       <c r="G14" s="68">
         <f>B14-J17</f>
         <v>12</v>
       </c>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="124"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="124"/>
-      <c r="V14" s="124"/>
-      <c r="W14" s="124"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="139"/>
+      <c r="L14" s="139"/>
+      <c r="M14" s="139"/>
+      <c r="N14" s="139"/>
+      <c r="O14" s="139"/>
+      <c r="P14" s="139"/>
+      <c r="Q14" s="139"/>
+      <c r="R14" s="139"/>
+      <c r="S14" s="139"/>
+      <c r="T14" s="139"/>
+      <c r="U14" s="139"/>
+      <c r="V14" s="139"/>
+      <c r="W14" s="139"/>
       <c r="X14" s="67"/>
     </row>
     <row r="15" spans="1:24" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131" t="s">
+      <c r="A15" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
-      <c r="I15" s="132"/>
-      <c r="J15" s="132"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="132"/>
-      <c r="M15" s="132"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
-      <c r="R15" s="132"/>
-      <c r="S15" s="132"/>
-      <c r="T15" s="132"/>
-      <c r="U15" s="132"/>
-      <c r="V15" s="132"/>
-      <c r="W15" s="132"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="131"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
+      <c r="P15" s="131"/>
+      <c r="Q15" s="131"/>
+      <c r="R15" s="131"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="131"/>
+      <c r="W15" s="131"/>
       <c r="X15" s="67"/>
     </row>
     <row r="16" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8363,31 +8363,31 @@
       <c r="X17" s="76"/>
     </row>
     <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="133" t="s">
+      <c r="A18" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="134"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="136"/>
-      <c r="I18" s="136"/>
-      <c r="J18" s="137"/>
-      <c r="K18" s="137"/>
-      <c r="L18" s="137"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="137"/>
-      <c r="T18" s="137"/>
-      <c r="U18" s="137"/>
-      <c r="V18" s="137"/>
-      <c r="W18" s="138"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="136"/>
+      <c r="M18" s="136"/>
+      <c r="N18" s="136"/>
+      <c r="O18" s="136"/>
+      <c r="P18" s="136"/>
+      <c r="Q18" s="136"/>
+      <c r="R18" s="136"/>
+      <c r="S18" s="136"/>
+      <c r="T18" s="136"/>
+      <c r="U18" s="136"/>
+      <c r="V18" s="136"/>
+      <c r="W18" s="137"/>
       <c r="X18" s="70"/>
     </row>
     <row r="19" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
@@ -8926,31 +8926,31 @@
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="139" t="s">
+      <c r="A26" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="140"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="140"/>
-      <c r="L26" s="140"/>
-      <c r="M26" s="140"/>
-      <c r="N26" s="140"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="140"/>
-      <c r="Q26" s="140"/>
-      <c r="R26" s="140"/>
-      <c r="S26" s="140"/>
-      <c r="T26" s="140"/>
-      <c r="U26" s="140"/>
-      <c r="V26" s="140"/>
-      <c r="W26" s="140"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="124"/>
+      <c r="U26" s="124"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="124"/>
       <c r="X26" s="70"/>
     </row>
     <row r="27" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
@@ -9399,31 +9399,31 @@
       <c r="Z32" s="94"/>
     </row>
     <row r="33" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="139" t="s">
+      <c r="A33" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="140"/>
-      <c r="C33" s="140"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="140"/>
-      <c r="J33" s="140"/>
-      <c r="K33" s="140"/>
-      <c r="L33" s="140"/>
-      <c r="M33" s="140"/>
-      <c r="N33" s="140"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="140"/>
-      <c r="Q33" s="140"/>
-      <c r="R33" s="140"/>
-      <c r="S33" s="140"/>
-      <c r="T33" s="140"/>
-      <c r="U33" s="140"/>
-      <c r="V33" s="140"/>
-      <c r="W33" s="140"/>
+      <c r="B33" s="124"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="124"/>
+      <c r="H33" s="124"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="124"/>
+      <c r="K33" s="124"/>
+      <c r="L33" s="124"/>
+      <c r="M33" s="124"/>
+      <c r="N33" s="124"/>
+      <c r="O33" s="124"/>
+      <c r="P33" s="124"/>
+      <c r="Q33" s="124"/>
+      <c r="R33" s="124"/>
+      <c r="S33" s="124"/>
+      <c r="T33" s="124"/>
+      <c r="U33" s="124"/>
+      <c r="V33" s="124"/>
+      <c r="W33" s="124"/>
       <c r="X33" s="70"/>
     </row>
     <row r="34" spans="1:24" ht="27.6" x14ac:dyDescent="0.3">
@@ -9835,29 +9835,29 @@
       <c r="X38" s="70"/>
     </row>
     <row r="39" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="146"/>
-      <c r="B39" s="140"/>
-      <c r="C39" s="140"/>
-      <c r="D39" s="140"/>
-      <c r="E39" s="140"/>
-      <c r="F39" s="140"/>
-      <c r="G39" s="140"/>
-      <c r="H39" s="140"/>
-      <c r="I39" s="140"/>
-      <c r="J39" s="140"/>
-      <c r="K39" s="140"/>
-      <c r="L39" s="140"/>
-      <c r="M39" s="140"/>
-      <c r="N39" s="140"/>
-      <c r="O39" s="140"/>
-      <c r="P39" s="140"/>
-      <c r="Q39" s="140"/>
-      <c r="R39" s="140"/>
-      <c r="S39" s="140"/>
-      <c r="T39" s="140"/>
-      <c r="U39" s="140"/>
-      <c r="V39" s="140"/>
-      <c r="W39" s="140"/>
+      <c r="A39" s="129"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="124"/>
+      <c r="E39" s="124"/>
+      <c r="F39" s="124"/>
+      <c r="G39" s="124"/>
+      <c r="H39" s="124"/>
+      <c r="I39" s="124"/>
+      <c r="J39" s="124"/>
+      <c r="K39" s="124"/>
+      <c r="L39" s="124"/>
+      <c r="M39" s="124"/>
+      <c r="N39" s="124"/>
+      <c r="O39" s="124"/>
+      <c r="P39" s="124"/>
+      <c r="Q39" s="124"/>
+      <c r="R39" s="124"/>
+      <c r="S39" s="124"/>
+      <c r="T39" s="124"/>
+      <c r="U39" s="124"/>
+      <c r="V39" s="124"/>
+      <c r="W39" s="124"/>
       <c r="X39" s="70"/>
     </row>
     <row r="40" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -9965,29 +9965,29 @@
       <c r="X43" s="70"/>
     </row>
     <row r="44" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="146"/>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="140"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="140"/>
-      <c r="Q44" s="140"/>
-      <c r="R44" s="140"/>
-      <c r="S44" s="140"/>
-      <c r="T44" s="140"/>
-      <c r="U44" s="140"/>
-      <c r="V44" s="140"/>
-      <c r="W44" s="140"/>
+      <c r="A44" s="129"/>
+      <c r="B44" s="124"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="124"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="124"/>
+      <c r="K44" s="124"/>
+      <c r="L44" s="124"/>
+      <c r="M44" s="124"/>
+      <c r="N44" s="124"/>
+      <c r="O44" s="124"/>
+      <c r="P44" s="124"/>
+      <c r="Q44" s="124"/>
+      <c r="R44" s="124"/>
+      <c r="S44" s="124"/>
+      <c r="T44" s="124"/>
+      <c r="U44" s="124"/>
+      <c r="V44" s="124"/>
+      <c r="W44" s="124"/>
       <c r="X44" s="70"/>
     </row>
     <row r="45" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -10043,29 +10043,29 @@
       <c r="X46" s="70"/>
     </row>
     <row r="47" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="146"/>
-      <c r="B47" s="140"/>
-      <c r="C47" s="140"/>
-      <c r="D47" s="140"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="140"/>
-      <c r="G47" s="140"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="140"/>
-      <c r="J47" s="140"/>
-      <c r="K47" s="140"/>
-      <c r="L47" s="140"/>
-      <c r="M47" s="140"/>
-      <c r="N47" s="140"/>
-      <c r="O47" s="140"/>
-      <c r="P47" s="140"/>
-      <c r="Q47" s="140"/>
-      <c r="R47" s="140"/>
-      <c r="S47" s="140"/>
-      <c r="T47" s="140"/>
-      <c r="U47" s="140"/>
-      <c r="V47" s="140"/>
-      <c r="W47" s="140"/>
+      <c r="A47" s="129"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="124"/>
+      <c r="D47" s="124"/>
+      <c r="E47" s="124"/>
+      <c r="F47" s="124"/>
+      <c r="G47" s="124"/>
+      <c r="H47" s="124"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="124"/>
+      <c r="K47" s="124"/>
+      <c r="L47" s="124"/>
+      <c r="M47" s="124"/>
+      <c r="N47" s="124"/>
+      <c r="O47" s="124"/>
+      <c r="P47" s="124"/>
+      <c r="Q47" s="124"/>
+      <c r="R47" s="124"/>
+      <c r="S47" s="124"/>
+      <c r="T47" s="124"/>
+      <c r="U47" s="124"/>
+      <c r="V47" s="124"/>
+      <c r="W47" s="124"/>
       <c r="X47" s="70"/>
     </row>
     <row r="48" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -10147,30 +10147,30 @@
       <c r="X50" s="70"/>
     </row>
     <row r="51" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="141"/>
-      <c r="B51" s="140"/>
-      <c r="C51" s="140"/>
-      <c r="D51" s="140"/>
-      <c r="E51" s="140"/>
-      <c r="F51" s="140"/>
-      <c r="G51" s="140"/>
-      <c r="H51" s="142"/>
-      <c r="I51" s="142"/>
-      <c r="J51" s="143"/>
-      <c r="K51" s="143"/>
-      <c r="L51" s="143"/>
-      <c r="M51" s="143"/>
-      <c r="N51" s="143"/>
-      <c r="O51" s="143"/>
-      <c r="P51" s="143"/>
-      <c r="Q51" s="143"/>
-      <c r="R51" s="143"/>
-      <c r="S51" s="143"/>
-      <c r="T51" s="143"/>
-      <c r="U51" s="143"/>
-      <c r="V51" s="143"/>
-      <c r="W51" s="144"/>
-      <c r="X51" s="145"/>
+      <c r="A51" s="123"/>
+      <c r="B51" s="124"/>
+      <c r="C51" s="124"/>
+      <c r="D51" s="124"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="124"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="126"/>
+      <c r="K51" s="126"/>
+      <c r="L51" s="126"/>
+      <c r="M51" s="126"/>
+      <c r="N51" s="126"/>
+      <c r="O51" s="126"/>
+      <c r="P51" s="126"/>
+      <c r="Q51" s="126"/>
+      <c r="R51" s="126"/>
+      <c r="S51" s="126"/>
+      <c r="T51" s="126"/>
+      <c r="U51" s="126"/>
+      <c r="V51" s="126"/>
+      <c r="W51" s="127"/>
+      <c r="X51" s="128"/>
     </row>
     <row r="52" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="81"/>
@@ -10199,30 +10199,30 @@
       <c r="X52" s="70"/>
     </row>
     <row r="53" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="141"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="140"/>
-      <c r="D53" s="140"/>
-      <c r="E53" s="140"/>
-      <c r="F53" s="140"/>
-      <c r="G53" s="140"/>
-      <c r="H53" s="142"/>
-      <c r="I53" s="142"/>
-      <c r="J53" s="143"/>
-      <c r="K53" s="143"/>
-      <c r="L53" s="143"/>
-      <c r="M53" s="143"/>
-      <c r="N53" s="143"/>
-      <c r="O53" s="143"/>
-      <c r="P53" s="143"/>
-      <c r="Q53" s="143"/>
-      <c r="R53" s="143"/>
-      <c r="S53" s="143"/>
-      <c r="T53" s="143"/>
-      <c r="U53" s="143"/>
-      <c r="V53" s="143"/>
-      <c r="W53" s="144"/>
-      <c r="X53" s="145"/>
+      <c r="A53" s="123"/>
+      <c r="B53" s="124"/>
+      <c r="C53" s="124"/>
+      <c r="D53" s="124"/>
+      <c r="E53" s="124"/>
+      <c r="F53" s="124"/>
+      <c r="G53" s="124"/>
+      <c r="H53" s="125"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="126"/>
+      <c r="K53" s="126"/>
+      <c r="L53" s="126"/>
+      <c r="M53" s="126"/>
+      <c r="N53" s="126"/>
+      <c r="O53" s="126"/>
+      <c r="P53" s="126"/>
+      <c r="Q53" s="126"/>
+      <c r="R53" s="126"/>
+      <c r="S53" s="126"/>
+      <c r="T53" s="126"/>
+      <c r="U53" s="126"/>
+      <c r="V53" s="126"/>
+      <c r="W53" s="127"/>
+      <c r="X53" s="128"/>
     </row>
     <row r="54" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="81"/>
@@ -10251,30 +10251,30 @@
       <c r="X54" s="70"/>
     </row>
     <row r="55" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="141"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="140"/>
-      <c r="D55" s="140"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="140"/>
-      <c r="H55" s="142"/>
-      <c r="I55" s="142"/>
-      <c r="J55" s="143"/>
-      <c r="K55" s="143"/>
-      <c r="L55" s="143"/>
-      <c r="M55" s="143"/>
-      <c r="N55" s="143"/>
-      <c r="O55" s="143"/>
-      <c r="P55" s="143"/>
-      <c r="Q55" s="143"/>
-      <c r="R55" s="143"/>
-      <c r="S55" s="143"/>
-      <c r="T55" s="143"/>
-      <c r="U55" s="143"/>
-      <c r="V55" s="143"/>
-      <c r="W55" s="144"/>
-      <c r="X55" s="145"/>
+      <c r="A55" s="123"/>
+      <c r="B55" s="124"/>
+      <c r="C55" s="124"/>
+      <c r="D55" s="124"/>
+      <c r="E55" s="124"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="124"/>
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="126"/>
+      <c r="K55" s="126"/>
+      <c r="L55" s="126"/>
+      <c r="M55" s="126"/>
+      <c r="N55" s="126"/>
+      <c r="O55" s="126"/>
+      <c r="P55" s="126"/>
+      <c r="Q55" s="126"/>
+      <c r="R55" s="126"/>
+      <c r="S55" s="126"/>
+      <c r="T55" s="126"/>
+      <c r="U55" s="126"/>
+      <c r="V55" s="126"/>
+      <c r="W55" s="127"/>
+      <c r="X55" s="128"/>
     </row>
     <row r="56" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="81"/>
@@ -11761,46 +11761,46 @@
     <row r="117" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:X2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:X3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:X9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:X10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:X11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:X12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:X13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:W14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="G15:W15"/>
+    <mergeCell ref="A18:W18"/>
+    <mergeCell ref="A26:W26"/>
+    <mergeCell ref="A33:W33"/>
     <mergeCell ref="A55:X55"/>
     <mergeCell ref="A39:W39"/>
     <mergeCell ref="A44:W44"/>
     <mergeCell ref="A47:W47"/>
     <mergeCell ref="A51:X51"/>
     <mergeCell ref="A53:X53"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="G15:W15"/>
-    <mergeCell ref="A18:W18"/>
-    <mergeCell ref="A26:W26"/>
-    <mergeCell ref="A33:W33"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:X13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:W14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:X10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:X11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:X12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:X9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:X6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:X1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:X2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11813,8 +11813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36:G37"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z43" sqref="Z43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11836,449 +11836,449 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="143" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
       <c r="D1" s="69">
         <v>2</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="139"/>
+      <c r="R1" s="139"/>
+      <c r="S1" s="139"/>
+      <c r="T1" s="139"/>
+      <c r="U1" s="139"/>
+      <c r="V1" s="139"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="139"/>
     </row>
     <row r="2" spans="1:24" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="139"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="139"/>
+      <c r="S2" s="139"/>
+      <c r="T2" s="139"/>
+      <c r="U2" s="139"/>
+      <c r="V2" s="139"/>
+      <c r="W2" s="139"/>
+      <c r="X2" s="139"/>
     </row>
     <row r="3" spans="1:24" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="128"/>
+      <c r="C3" s="146"/>
       <c r="D3" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="129" t="s">
+      <c r="E3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="129"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="129"/>
-      <c r="S3" s="129"/>
-      <c r="T3" s="129"/>
-      <c r="U3" s="129"/>
-      <c r="V3" s="129"/>
-      <c r="W3" s="129"/>
-      <c r="X3" s="129"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="141"/>
+      <c r="O3" s="141"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="141"/>
+      <c r="T3" s="141"/>
+      <c r="U3" s="141"/>
+      <c r="V3" s="141"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="141"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="102">
         <v>1</v>
       </c>
-      <c r="B4" s="127">
+      <c r="B4" s="142">
         <v>20</v>
       </c>
-      <c r="C4" s="127"/>
+      <c r="C4" s="142"/>
       <c r="D4" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="124"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="139"/>
+      <c r="T4" s="139"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="100">
         <v>2</v>
       </c>
-      <c r="B5" s="127">
+      <c r="B5" s="142">
         <v>20</v>
       </c>
-      <c r="C5" s="127"/>
+      <c r="C5" s="142"/>
       <c r="D5" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="139"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="139"/>
+      <c r="S5" s="139"/>
+      <c r="T5" s="139"/>
+      <c r="U5" s="139"/>
+      <c r="V5" s="139"/>
+      <c r="W5" s="139"/>
+      <c r="X5" s="139"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="100">
         <v>3</v>
       </c>
-      <c r="B6" s="124">
+      <c r="B6" s="139">
         <v>20</v>
       </c>
-      <c r="C6" s="124"/>
+      <c r="C6" s="139"/>
       <c r="D6" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="127"/>
-      <c r="U6" s="127"/>
-      <c r="V6" s="127"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="127"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
+      <c r="J6" s="142"/>
+      <c r="K6" s="142"/>
+      <c r="L6" s="142"/>
+      <c r="M6" s="142"/>
+      <c r="N6" s="142"/>
+      <c r="O6" s="142"/>
+      <c r="P6" s="142"/>
+      <c r="Q6" s="142"/>
+      <c r="R6" s="142"/>
+      <c r="S6" s="142"/>
+      <c r="T6" s="142"/>
+      <c r="U6" s="142"/>
+      <c r="V6" s="142"/>
+      <c r="W6" s="142"/>
+      <c r="X6" s="142"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100">
         <v>4</v>
       </c>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
       <c r="D7" s="102"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
-      <c r="T7" s="127"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="127"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="127"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="142"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
+      <c r="V7" s="142"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="142"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="100">
         <v>5</v>
       </c>
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
       <c r="D8" s="100"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="127"/>
-      <c r="P8" s="127"/>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="127"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="127"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
+      <c r="H8" s="142"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="142"/>
+      <c r="M8" s="142"/>
+      <c r="N8" s="142"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="142"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="142"/>
+      <c r="S8" s="142"/>
+      <c r="T8" s="142"/>
+      <c r="U8" s="142"/>
+      <c r="V8" s="142"/>
+      <c r="W8" s="142"/>
+      <c r="X8" s="142"/>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="100">
         <v>6</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="124"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
       <c r="D9" s="100"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="124"/>
-      <c r="X9" s="124"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="139"/>
+      <c r="O9" s="139"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="139"/>
+      <c r="S9" s="139"/>
+      <c r="T9" s="139"/>
+      <c r="U9" s="139"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="139"/>
+      <c r="X9" s="139"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100">
         <v>7</v>
       </c>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
       <c r="D10" s="100"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="124"/>
-      <c r="Q10" s="124"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="124"/>
-      <c r="T10" s="124"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="124"/>
-      <c r="W10" s="124"/>
-      <c r="X10" s="124"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="139"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="139"/>
+      <c r="M10" s="139"/>
+      <c r="N10" s="139"/>
+      <c r="O10" s="139"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="139"/>
+      <c r="R10" s="139"/>
+      <c r="S10" s="139"/>
+      <c r="T10" s="139"/>
+      <c r="U10" s="139"/>
+      <c r="V10" s="139"/>
+      <c r="W10" s="139"/>
+      <c r="X10" s="139"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="100">
         <v>8</v>
       </c>
-      <c r="B11" s="124"/>
-      <c r="C11" s="124"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="100"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-      <c r="Q11" s="124"/>
-      <c r="R11" s="124"/>
-      <c r="S11" s="124"/>
-      <c r="T11" s="124"/>
-      <c r="U11" s="124"/>
-      <c r="V11" s="124"/>
-      <c r="W11" s="124"/>
-      <c r="X11" s="124"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="139"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="139"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="139"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="139"/>
+      <c r="N11" s="139"/>
+      <c r="O11" s="139"/>
+      <c r="P11" s="139"/>
+      <c r="Q11" s="139"/>
+      <c r="R11" s="139"/>
+      <c r="S11" s="139"/>
+      <c r="T11" s="139"/>
+      <c r="U11" s="139"/>
+      <c r="V11" s="139"/>
+      <c r="W11" s="139"/>
+      <c r="X11" s="139"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="100">
         <v>9</v>
       </c>
-      <c r="B12" s="124"/>
-      <c r="C12" s="124"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="100"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-      <c r="Q12" s="124"/>
-      <c r="R12" s="124"/>
-      <c r="S12" s="124"/>
-      <c r="T12" s="124"/>
-      <c r="U12" s="124"/>
-      <c r="V12" s="124"/>
-      <c r="W12" s="124"/>
-      <c r="X12" s="124"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="139"/>
+      <c r="N12" s="139"/>
+      <c r="O12" s="139"/>
+      <c r="P12" s="139"/>
+      <c r="Q12" s="139"/>
+      <c r="R12" s="139"/>
+      <c r="S12" s="139"/>
+      <c r="T12" s="139"/>
+      <c r="U12" s="139"/>
+      <c r="V12" s="139"/>
+      <c r="W12" s="139"/>
+      <c r="X12" s="139"/>
     </row>
     <row r="13" spans="1:24" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="100">
         <v>10</v>
       </c>
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
       <c r="D13" s="100"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-      <c r="Q13" s="124"/>
-      <c r="R13" s="124"/>
-      <c r="S13" s="124"/>
-      <c r="T13" s="124"/>
-      <c r="U13" s="124"/>
-      <c r="V13" s="124"/>
-      <c r="W13" s="124"/>
-      <c r="X13" s="124"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="139"/>
+      <c r="N13" s="139"/>
+      <c r="O13" s="139"/>
+      <c r="P13" s="139"/>
+      <c r="Q13" s="139"/>
+      <c r="R13" s="139"/>
+      <c r="S13" s="139"/>
+      <c r="T13" s="139"/>
+      <c r="U13" s="139"/>
+      <c r="V13" s="139"/>
+      <c r="W13" s="139"/>
+      <c r="X13" s="139"/>
     </row>
     <row r="14" spans="1:24" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="100"/>
-      <c r="B14" s="130">
+      <c r="B14" s="140">
         <f>SUM(B4:C13)</f>
         <v>60</v>
       </c>
-      <c r="C14" s="130"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="100"/>
-      <c r="E14" s="129" t="s">
+      <c r="E14" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="129"/>
+      <c r="F14" s="141"/>
       <c r="G14" s="101">
         <f>B14-J17</f>
         <v>21</v>
       </c>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="124"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="124"/>
-      <c r="V14" s="124"/>
-      <c r="W14" s="124"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="139"/>
+      <c r="L14" s="139"/>
+      <c r="M14" s="139"/>
+      <c r="N14" s="139"/>
+      <c r="O14" s="139"/>
+      <c r="P14" s="139"/>
+      <c r="Q14" s="139"/>
+      <c r="R14" s="139"/>
+      <c r="S14" s="139"/>
+      <c r="T14" s="139"/>
+      <c r="U14" s="139"/>
+      <c r="V14" s="139"/>
+      <c r="W14" s="139"/>
       <c r="X14" s="100"/>
     </row>
     <row r="15" spans="1:24" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131" t="s">
+      <c r="A15" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
-      <c r="I15" s="132"/>
-      <c r="J15" s="132"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="132"/>
-      <c r="M15" s="132"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
-      <c r="R15" s="132"/>
-      <c r="S15" s="132"/>
-      <c r="T15" s="132"/>
-      <c r="U15" s="132"/>
-      <c r="V15" s="132"/>
-      <c r="W15" s="132"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="131"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
+      <c r="P15" s="131"/>
+      <c r="Q15" s="131"/>
+      <c r="R15" s="131"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="131"/>
+      <c r="W15" s="131"/>
       <c r="X15" s="100"/>
     </row>
     <row r="16" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12422,31 +12422,31 @@
       <c r="X17" s="76"/>
     </row>
     <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="133" t="s">
+      <c r="A18" s="132" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="134"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="136"/>
-      <c r="I18" s="136"/>
-      <c r="J18" s="137"/>
-      <c r="K18" s="137"/>
-      <c r="L18" s="137"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="137"/>
-      <c r="T18" s="137"/>
-      <c r="U18" s="137"/>
-      <c r="V18" s="137"/>
-      <c r="W18" s="138"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="136"/>
+      <c r="M18" s="136"/>
+      <c r="N18" s="136"/>
+      <c r="O18" s="136"/>
+      <c r="P18" s="136"/>
+      <c r="Q18" s="136"/>
+      <c r="R18" s="136"/>
+      <c r="S18" s="136"/>
+      <c r="T18" s="136"/>
+      <c r="U18" s="136"/>
+      <c r="V18" s="136"/>
+      <c r="W18" s="137"/>
       <c r="X18" s="70"/>
     </row>
     <row r="19" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
@@ -12971,31 +12971,31 @@
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="139" t="s">
+      <c r="A26" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="140"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="140"/>
-      <c r="L26" s="140"/>
-      <c r="M26" s="140"/>
-      <c r="N26" s="140"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="140"/>
-      <c r="Q26" s="140"/>
-      <c r="R26" s="140"/>
-      <c r="S26" s="140"/>
-      <c r="T26" s="140"/>
-      <c r="U26" s="140"/>
-      <c r="V26" s="140"/>
-      <c r="W26" s="140"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="124"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
+      <c r="P26" s="124"/>
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="124"/>
+      <c r="U26" s="124"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="124"/>
       <c r="X26" s="70"/>
     </row>
     <row r="27" spans="1:26" ht="41.4" x14ac:dyDescent="0.3">
@@ -13017,8 +13017,8 @@
       <c r="F27" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="87" t="s">
-        <v>63</v>
+      <c r="G27" s="157" t="s">
+        <v>111</v>
       </c>
       <c r="H27" s="83">
         <v>15</v>
@@ -13103,8 +13103,8 @@
       <c r="F28" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="G28" s="87" t="s">
-        <v>63</v>
+      <c r="G28" s="157" t="s">
+        <v>111</v>
       </c>
       <c r="H28" s="83">
         <v>2</v>
@@ -13430,31 +13430,31 @@
       <c r="Z32" s="94"/>
     </row>
     <row r="33" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="139" t="s">
+      <c r="A33" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="140"/>
-      <c r="C33" s="140"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="140"/>
-      <c r="J33" s="140"/>
-      <c r="K33" s="140"/>
-      <c r="L33" s="140"/>
-      <c r="M33" s="140"/>
-      <c r="N33" s="140"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="140"/>
-      <c r="Q33" s="140"/>
-      <c r="R33" s="140"/>
-      <c r="S33" s="140"/>
-      <c r="T33" s="140"/>
-      <c r="U33" s="140"/>
-      <c r="V33" s="140"/>
-      <c r="W33" s="140"/>
+      <c r="B33" s="124"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="124"/>
+      <c r="H33" s="124"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="124"/>
+      <c r="K33" s="124"/>
+      <c r="L33" s="124"/>
+      <c r="M33" s="124"/>
+      <c r="N33" s="124"/>
+      <c r="O33" s="124"/>
+      <c r="P33" s="124"/>
+      <c r="Q33" s="124"/>
+      <c r="R33" s="124"/>
+      <c r="S33" s="124"/>
+      <c r="T33" s="124"/>
+      <c r="U33" s="124"/>
+      <c r="V33" s="124"/>
+      <c r="W33" s="124"/>
       <c r="X33" s="70"/>
     </row>
     <row r="34" spans="1:24" ht="27.6" x14ac:dyDescent="0.3">
@@ -13734,8 +13734,8 @@
       <c r="F37" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="G37" s="87" t="s">
-        <v>63</v>
+      <c r="G37" s="157" t="s">
+        <v>111</v>
       </c>
       <c r="H37" s="83">
         <v>4</v>
@@ -13813,10 +13813,16 @@
         <f>IF(ISBLANK(B38),"",CONCATENATE("ID",A38,"-",B38))</f>
         <v>ID2-3</v>
       </c>
-      <c r="D38" s="81"/>
+      <c r="D38" s="97" t="s">
+        <v>110</v>
+      </c>
       <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="99"/>
+      <c r="F38" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="157" t="s">
+        <v>111</v>
+      </c>
       <c r="H38" s="83"/>
       <c r="I38" s="84">
         <f>W38</f>
@@ -13880,29 +13886,29 @@
       <c r="X38" s="70"/>
     </row>
     <row r="39" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="146"/>
-      <c r="B39" s="140"/>
-      <c r="C39" s="140"/>
-      <c r="D39" s="140"/>
-      <c r="E39" s="140"/>
-      <c r="F39" s="140"/>
-      <c r="G39" s="140"/>
-      <c r="H39" s="140"/>
-      <c r="I39" s="140"/>
-      <c r="J39" s="140"/>
-      <c r="K39" s="140"/>
-      <c r="L39" s="140"/>
-      <c r="M39" s="140"/>
-      <c r="N39" s="140"/>
-      <c r="O39" s="140"/>
-      <c r="P39" s="140"/>
-      <c r="Q39" s="140"/>
-      <c r="R39" s="140"/>
-      <c r="S39" s="140"/>
-      <c r="T39" s="140"/>
-      <c r="U39" s="140"/>
-      <c r="V39" s="140"/>
-      <c r="W39" s="140"/>
+      <c r="A39" s="129"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="124"/>
+      <c r="E39" s="124"/>
+      <c r="F39" s="124"/>
+      <c r="G39" s="124"/>
+      <c r="H39" s="124"/>
+      <c r="I39" s="124"/>
+      <c r="J39" s="124"/>
+      <c r="K39" s="124"/>
+      <c r="L39" s="124"/>
+      <c r="M39" s="124"/>
+      <c r="N39" s="124"/>
+      <c r="O39" s="124"/>
+      <c r="P39" s="124"/>
+      <c r="Q39" s="124"/>
+      <c r="R39" s="124"/>
+      <c r="S39" s="124"/>
+      <c r="T39" s="124"/>
+      <c r="U39" s="124"/>
+      <c r="V39" s="124"/>
+      <c r="W39" s="124"/>
       <c r="X39" s="70"/>
     </row>
     <row r="40" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -14010,29 +14016,29 @@
       <c r="X43" s="70"/>
     </row>
     <row r="44" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="146"/>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="140"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="140"/>
-      <c r="Q44" s="140"/>
-      <c r="R44" s="140"/>
-      <c r="S44" s="140"/>
-      <c r="T44" s="140"/>
-      <c r="U44" s="140"/>
-      <c r="V44" s="140"/>
-      <c r="W44" s="140"/>
+      <c r="A44" s="129"/>
+      <c r="B44" s="124"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="124"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="124"/>
+      <c r="K44" s="124"/>
+      <c r="L44" s="124"/>
+      <c r="M44" s="124"/>
+      <c r="N44" s="124"/>
+      <c r="O44" s="124"/>
+      <c r="P44" s="124"/>
+      <c r="Q44" s="124"/>
+      <c r="R44" s="124"/>
+      <c r="S44" s="124"/>
+      <c r="T44" s="124"/>
+      <c r="U44" s="124"/>
+      <c r="V44" s="124"/>
+      <c r="W44" s="124"/>
       <c r="X44" s="70"/>
     </row>
     <row r="45" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -14088,29 +14094,29 @@
       <c r="X46" s="70"/>
     </row>
     <row r="47" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="146"/>
-      <c r="B47" s="140"/>
-      <c r="C47" s="140"/>
-      <c r="D47" s="140"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="140"/>
-      <c r="G47" s="140"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="140"/>
-      <c r="J47" s="140"/>
-      <c r="K47" s="140"/>
-      <c r="L47" s="140"/>
-      <c r="M47" s="140"/>
-      <c r="N47" s="140"/>
-      <c r="O47" s="140"/>
-      <c r="P47" s="140"/>
-      <c r="Q47" s="140"/>
-      <c r="R47" s="140"/>
-      <c r="S47" s="140"/>
-      <c r="T47" s="140"/>
-      <c r="U47" s="140"/>
-      <c r="V47" s="140"/>
-      <c r="W47" s="140"/>
+      <c r="A47" s="129"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="124"/>
+      <c r="D47" s="124"/>
+      <c r="E47" s="124"/>
+      <c r="F47" s="124"/>
+      <c r="G47" s="124"/>
+      <c r="H47" s="124"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="124"/>
+      <c r="K47" s="124"/>
+      <c r="L47" s="124"/>
+      <c r="M47" s="124"/>
+      <c r="N47" s="124"/>
+      <c r="O47" s="124"/>
+      <c r="P47" s="124"/>
+      <c r="Q47" s="124"/>
+      <c r="R47" s="124"/>
+      <c r="S47" s="124"/>
+      <c r="T47" s="124"/>
+      <c r="U47" s="124"/>
+      <c r="V47" s="124"/>
+      <c r="W47" s="124"/>
       <c r="X47" s="70"/>
     </row>
     <row r="48" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
@@ -14192,30 +14198,30 @@
       <c r="X50" s="70"/>
     </row>
     <row r="51" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="141"/>
-      <c r="B51" s="140"/>
-      <c r="C51" s="140"/>
-      <c r="D51" s="140"/>
-      <c r="E51" s="140"/>
-      <c r="F51" s="140"/>
-      <c r="G51" s="140"/>
-      <c r="H51" s="142"/>
-      <c r="I51" s="142"/>
-      <c r="J51" s="143"/>
-      <c r="K51" s="143"/>
-      <c r="L51" s="143"/>
-      <c r="M51" s="143"/>
-      <c r="N51" s="143"/>
-      <c r="O51" s="143"/>
-      <c r="P51" s="143"/>
-      <c r="Q51" s="143"/>
-      <c r="R51" s="143"/>
-      <c r="S51" s="143"/>
-      <c r="T51" s="143"/>
-      <c r="U51" s="143"/>
-      <c r="V51" s="143"/>
-      <c r="W51" s="144"/>
-      <c r="X51" s="145"/>
+      <c r="A51" s="123"/>
+      <c r="B51" s="124"/>
+      <c r="C51" s="124"/>
+      <c r="D51" s="124"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="124"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="126"/>
+      <c r="K51" s="126"/>
+      <c r="L51" s="126"/>
+      <c r="M51" s="126"/>
+      <c r="N51" s="126"/>
+      <c r="O51" s="126"/>
+      <c r="P51" s="126"/>
+      <c r="Q51" s="126"/>
+      <c r="R51" s="126"/>
+      <c r="S51" s="126"/>
+      <c r="T51" s="126"/>
+      <c r="U51" s="126"/>
+      <c r="V51" s="126"/>
+      <c r="W51" s="127"/>
+      <c r="X51" s="128"/>
     </row>
     <row r="52" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="81"/>
@@ -14244,30 +14250,30 @@
       <c r="X52" s="70"/>
     </row>
     <row r="53" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="141"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="140"/>
-      <c r="D53" s="140"/>
-      <c r="E53" s="140"/>
-      <c r="F53" s="140"/>
-      <c r="G53" s="140"/>
-      <c r="H53" s="142"/>
-      <c r="I53" s="142"/>
-      <c r="J53" s="143"/>
-      <c r="K53" s="143"/>
-      <c r="L53" s="143"/>
-      <c r="M53" s="143"/>
-      <c r="N53" s="143"/>
-      <c r="O53" s="143"/>
-      <c r="P53" s="143"/>
-      <c r="Q53" s="143"/>
-      <c r="R53" s="143"/>
-      <c r="S53" s="143"/>
-      <c r="T53" s="143"/>
-      <c r="U53" s="143"/>
-      <c r="V53" s="143"/>
-      <c r="W53" s="144"/>
-      <c r="X53" s="145"/>
+      <c r="A53" s="123"/>
+      <c r="B53" s="124"/>
+      <c r="C53" s="124"/>
+      <c r="D53" s="124"/>
+      <c r="E53" s="124"/>
+      <c r="F53" s="124"/>
+      <c r="G53" s="124"/>
+      <c r="H53" s="125"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="126"/>
+      <c r="K53" s="126"/>
+      <c r="L53" s="126"/>
+      <c r="M53" s="126"/>
+      <c r="N53" s="126"/>
+      <c r="O53" s="126"/>
+      <c r="P53" s="126"/>
+      <c r="Q53" s="126"/>
+      <c r="R53" s="126"/>
+      <c r="S53" s="126"/>
+      <c r="T53" s="126"/>
+      <c r="U53" s="126"/>
+      <c r="V53" s="126"/>
+      <c r="W53" s="127"/>
+      <c r="X53" s="128"/>
     </row>
     <row r="54" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="81"/>
@@ -14296,30 +14302,30 @@
       <c r="X54" s="70"/>
     </row>
     <row r="55" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="141"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="140"/>
-      <c r="D55" s="140"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="140"/>
-      <c r="H55" s="142"/>
-      <c r="I55" s="142"/>
-      <c r="J55" s="143"/>
-      <c r="K55" s="143"/>
-      <c r="L55" s="143"/>
-      <c r="M55" s="143"/>
-      <c r="N55" s="143"/>
-      <c r="O55" s="143"/>
-      <c r="P55" s="143"/>
-      <c r="Q55" s="143"/>
-      <c r="R55" s="143"/>
-      <c r="S55" s="143"/>
-      <c r="T55" s="143"/>
-      <c r="U55" s="143"/>
-      <c r="V55" s="143"/>
-      <c r="W55" s="144"/>
-      <c r="X55" s="145"/>
+      <c r="A55" s="123"/>
+      <c r="B55" s="124"/>
+      <c r="C55" s="124"/>
+      <c r="D55" s="124"/>
+      <c r="E55" s="124"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="124"/>
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="126"/>
+      <c r="K55" s="126"/>
+      <c r="L55" s="126"/>
+      <c r="M55" s="126"/>
+      <c r="N55" s="126"/>
+      <c r="O55" s="126"/>
+      <c r="P55" s="126"/>
+      <c r="Q55" s="126"/>
+      <c r="R55" s="126"/>
+      <c r="S55" s="126"/>
+      <c r="T55" s="126"/>
+      <c r="U55" s="126"/>
+      <c r="V55" s="126"/>
+      <c r="W55" s="127"/>
+      <c r="X55" s="128"/>
     </row>
     <row r="56" spans="1:24" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="81"/>
@@ -15806,6 +15812,37 @@
     <row r="117" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:X2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:X3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:X9"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="G15:W15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:X10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:X11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:X12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:X13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:W14"/>
     <mergeCell ref="A51:X51"/>
     <mergeCell ref="A53:X53"/>
     <mergeCell ref="A55:X55"/>
@@ -15815,37 +15852,6 @@
     <mergeCell ref="A39:W39"/>
     <mergeCell ref="A44:W44"/>
     <mergeCell ref="A47:W47"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:X13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:W14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="G15:W15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:X10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:X11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:X12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:X9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:X6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:X1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:X2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -15877,437 +15883,437 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
       <c r="D1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="148"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="148"/>
-      <c r="P1" s="148"/>
-      <c r="Q1" s="148"/>
-      <c r="R1" s="148"/>
-      <c r="S1" s="148"/>
-      <c r="T1" s="148"/>
-      <c r="U1" s="148"/>
-      <c r="V1" s="148"/>
-      <c r="W1" s="148"/>
-      <c r="X1" s="148"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
+      <c r="M1" s="149"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="149"/>
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
+      <c r="U1" s="149"/>
+      <c r="V1" s="149"/>
+      <c r="W1" s="149"/>
+      <c r="X1" s="149"/>
     </row>
     <row r="2" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
-      <c r="U2" s="148"/>
-      <c r="V2" s="148"/>
-      <c r="W2" s="148"/>
-      <c r="X2" s="148"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
+      <c r="O2" s="149"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="149"/>
+      <c r="U2" s="149"/>
+      <c r="V2" s="149"/>
+      <c r="W2" s="149"/>
+      <c r="X2" s="149"/>
     </row>
     <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="156"/>
       <c r="D3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="155" t="s">
+      <c r="E3" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
-      <c r="K3" s="155"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="155"/>
-      <c r="O3" s="155"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="155"/>
-      <c r="R3" s="155"/>
-      <c r="S3" s="155"/>
-      <c r="T3" s="155"/>
-      <c r="U3" s="155"/>
-      <c r="V3" s="155"/>
-      <c r="W3" s="155"/>
-      <c r="X3" s="155"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="151"/>
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="151"/>
+      <c r="R3" s="151"/>
+      <c r="S3" s="151"/>
+      <c r="T3" s="151"/>
+      <c r="U3" s="151"/>
+      <c r="V3" s="151"/>
+      <c r="W3" s="151"/>
+      <c r="X3" s="151"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
         <v>1</v>
       </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
       <c r="D4" s="50"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="148"/>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
-      <c r="U4" s="148"/>
-      <c r="V4" s="148"/>
-      <c r="W4" s="148"/>
-      <c r="X4" s="148"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="149"/>
+      <c r="G4" s="149"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="149"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="149"/>
+      <c r="N4" s="149"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="149"/>
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="149"/>
+      <c r="V4" s="149"/>
+      <c r="W4" s="149"/>
+      <c r="X4" s="149"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>2</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="153"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="152"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="148"/>
-      <c r="K5" s="148"/>
-      <c r="L5" s="148"/>
-      <c r="M5" s="148"/>
-      <c r="N5" s="148"/>
-      <c r="O5" s="148"/>
-      <c r="P5" s="148"/>
-      <c r="Q5" s="148"/>
-      <c r="R5" s="148"/>
-      <c r="S5" s="148"/>
-      <c r="T5" s="148"/>
-      <c r="U5" s="148"/>
-      <c r="V5" s="148"/>
-      <c r="W5" s="148"/>
-      <c r="X5" s="148"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
+      <c r="M5" s="149"/>
+      <c r="N5" s="149"/>
+      <c r="O5" s="149"/>
+      <c r="P5" s="149"/>
+      <c r="Q5" s="149"/>
+      <c r="R5" s="149"/>
+      <c r="S5" s="149"/>
+      <c r="T5" s="149"/>
+      <c r="U5" s="149"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
+      <c r="X5" s="149"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>3</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="149"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="153"/>
-      <c r="M6" s="153"/>
-      <c r="N6" s="153"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="153"/>
-      <c r="Q6" s="153"/>
-      <c r="R6" s="153"/>
-      <c r="S6" s="153"/>
-      <c r="T6" s="153"/>
-      <c r="U6" s="153"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="153"/>
-      <c r="X6" s="153"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
+      <c r="H6" s="152"/>
+      <c r="I6" s="152"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="152"/>
+      <c r="M6" s="152"/>
+      <c r="N6" s="152"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
+      <c r="R6" s="152"/>
+      <c r="S6" s="152"/>
+      <c r="T6" s="152"/>
+      <c r="U6" s="152"/>
+      <c r="V6" s="152"/>
+      <c r="W6" s="152"/>
+      <c r="X6" s="152"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>4</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="148"/>
+      <c r="B7" s="149"/>
+      <c r="C7" s="149"/>
       <c r="D7" s="50"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="153"/>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
-      <c r="T7" s="153"/>
-      <c r="U7" s="153"/>
-      <c r="V7" s="153"/>
-      <c r="W7" s="153"/>
-      <c r="X7" s="153"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="152"/>
+      <c r="J7" s="152"/>
+      <c r="K7" s="152"/>
+      <c r="L7" s="152"/>
+      <c r="M7" s="152"/>
+      <c r="N7" s="152"/>
+      <c r="O7" s="152"/>
+      <c r="P7" s="152"/>
+      <c r="Q7" s="152"/>
+      <c r="R7" s="152"/>
+      <c r="S7" s="152"/>
+      <c r="T7" s="152"/>
+      <c r="U7" s="152"/>
+      <c r="V7" s="152"/>
+      <c r="W7" s="152"/>
+      <c r="X7" s="152"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>5</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="153"/>
-      <c r="O8" s="153"/>
-      <c r="P8" s="153"/>
-      <c r="Q8" s="153"/>
-      <c r="R8" s="153"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="153"/>
-      <c r="U8" s="153"/>
-      <c r="V8" s="153"/>
-      <c r="W8" s="153"/>
-      <c r="X8" s="153"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="152"/>
+      <c r="K8" s="152"/>
+      <c r="L8" s="152"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="152"/>
+      <c r="O8" s="152"/>
+      <c r="P8" s="152"/>
+      <c r="Q8" s="152"/>
+      <c r="R8" s="152"/>
+      <c r="S8" s="152"/>
+      <c r="T8" s="152"/>
+      <c r="U8" s="152"/>
+      <c r="V8" s="152"/>
+      <c r="W8" s="152"/>
+      <c r="X8" s="152"/>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>6</v>
       </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="149"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="148"/>
-      <c r="T9" s="148"/>
-      <c r="U9" s="148"/>
-      <c r="V9" s="148"/>
-      <c r="W9" s="148"/>
-      <c r="X9" s="148"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="149"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="149"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="149"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="149"/>
+      <c r="T9" s="149"/>
+      <c r="U9" s="149"/>
+      <c r="V9" s="149"/>
+      <c r="W9" s="149"/>
+      <c r="X9" s="149"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>7</v>
       </c>
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
+      <c r="B10" s="149"/>
+      <c r="C10" s="149"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="148"/>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="148"/>
-      <c r="P10" s="148"/>
-      <c r="Q10" s="148"/>
-      <c r="R10" s="148"/>
-      <c r="S10" s="148"/>
-      <c r="T10" s="148"/>
-      <c r="U10" s="148"/>
-      <c r="V10" s="148"/>
-      <c r="W10" s="148"/>
-      <c r="X10" s="148"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="149"/>
+      <c r="N10" s="149"/>
+      <c r="O10" s="149"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="149"/>
+      <c r="T10" s="149"/>
+      <c r="U10" s="149"/>
+      <c r="V10" s="149"/>
+      <c r="W10" s="149"/>
+      <c r="X10" s="149"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>8</v>
       </c>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="149"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="148"/>
-      <c r="I11" s="148"/>
-      <c r="J11" s="148"/>
-      <c r="K11" s="148"/>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
-      <c r="N11" s="148"/>
-      <c r="O11" s="148"/>
-      <c r="P11" s="148"/>
-      <c r="Q11" s="148"/>
-      <c r="R11" s="148"/>
-      <c r="S11" s="148"/>
-      <c r="T11" s="148"/>
-      <c r="U11" s="148"/>
-      <c r="V11" s="148"/>
-      <c r="W11" s="148"/>
-      <c r="X11" s="148"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
+      <c r="K11" s="149"/>
+      <c r="L11" s="149"/>
+      <c r="M11" s="149"/>
+      <c r="N11" s="149"/>
+      <c r="O11" s="149"/>
+      <c r="P11" s="149"/>
+      <c r="Q11" s="149"/>
+      <c r="R11" s="149"/>
+      <c r="S11" s="149"/>
+      <c r="T11" s="149"/>
+      <c r="U11" s="149"/>
+      <c r="V11" s="149"/>
+      <c r="W11" s="149"/>
+      <c r="X11" s="149"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>9</v>
       </c>
-      <c r="B12" s="148"/>
-      <c r="C12" s="148"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="148"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="148"/>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
-      <c r="X12" s="148"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="149"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="149"/>
+      <c r="L12" s="149"/>
+      <c r="M12" s="149"/>
+      <c r="N12" s="149"/>
+      <c r="O12" s="149"/>
+      <c r="P12" s="149"/>
+      <c r="Q12" s="149"/>
+      <c r="R12" s="149"/>
+      <c r="S12" s="149"/>
+      <c r="T12" s="149"/>
+      <c r="U12" s="149"/>
+      <c r="V12" s="149"/>
+      <c r="W12" s="149"/>
+      <c r="X12" s="149"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>10</v>
       </c>
-      <c r="B13" s="148"/>
-      <c r="C13" s="148"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="149"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="148"/>
-      <c r="U13" s="148"/>
-      <c r="V13" s="148"/>
-      <c r="W13" s="148"/>
-      <c r="X13" s="148"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="149"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149"/>
+      <c r="M13" s="149"/>
+      <c r="N13" s="149"/>
+      <c r="O13" s="149"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="149"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="149"/>
+      <c r="U13" s="149"/>
+      <c r="V13" s="149"/>
+      <c r="W13" s="149"/>
+      <c r="X13" s="149"/>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25"/>
-      <c r="B14" s="156">
+      <c r="B14" s="150">
         <f>SUM(B4:C13)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="156"/>
+      <c r="C14" s="150"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="155" t="s">
+      <c r="E14" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="155"/>
+      <c r="F14" s="151"/>
       <c r="G14" s="49">
         <f>B14-J17</f>
         <v>0</v>
       </c>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="148"/>
-      <c r="O14" s="148"/>
-      <c r="P14" s="148"/>
-      <c r="Q14" s="148"/>
-      <c r="R14" s="148"/>
-      <c r="S14" s="148"/>
-      <c r="T14" s="148"/>
-      <c r="U14" s="148"/>
-      <c r="V14" s="148"/>
-      <c r="W14" s="148"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="149"/>
+      <c r="L14" s="149"/>
+      <c r="M14" s="149"/>
+      <c r="N14" s="149"/>
+      <c r="O14" s="149"/>
+      <c r="P14" s="149"/>
+      <c r="Q14" s="149"/>
+      <c r="R14" s="149"/>
+      <c r="S14" s="149"/>
+      <c r="T14" s="149"/>
+      <c r="U14" s="149"/>
+      <c r="V14" s="149"/>
+      <c r="W14" s="149"/>
       <c r="X14" s="25"/>
     </row>
     <row r="15" spans="1:24" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="149"/>
-      <c r="F15" s="149"/>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="150"/>
-      <c r="L15" s="150"/>
-      <c r="M15" s="150"/>
-      <c r="N15" s="150"/>
-      <c r="O15" s="150"/>
-      <c r="P15" s="150"/>
-      <c r="Q15" s="150"/>
-      <c r="R15" s="150"/>
-      <c r="S15" s="150"/>
-      <c r="T15" s="150"/>
-      <c r="U15" s="150"/>
-      <c r="V15" s="150"/>
-      <c r="W15" s="150"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="148"/>
+      <c r="I15" s="148"/>
+      <c r="J15" s="148"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="148"/>
+      <c r="N15" s="148"/>
+      <c r="O15" s="148"/>
+      <c r="P15" s="148"/>
+      <c r="Q15" s="148"/>
+      <c r="R15" s="148"/>
+      <c r="S15" s="148"/>
+      <c r="T15" s="148"/>
+      <c r="U15" s="148"/>
+      <c r="V15" s="148"/>
+      <c r="W15" s="148"/>
       <c r="X15" s="25"/>
     </row>
     <row r="16" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -24431,6 +24437,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:X2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:X3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:X9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:X10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:X11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:X12"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="G15:W15"/>
     <mergeCell ref="B13:C13"/>
@@ -24438,30 +24468,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="H14:W14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:X10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:X11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:X12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:X9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:X6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:X1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:X2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24492,437 +24498,437 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
       <c r="D1" s="37">
         <v>1</v>
       </c>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="148"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="148"/>
-      <c r="P1" s="148"/>
-      <c r="Q1" s="148"/>
-      <c r="R1" s="148"/>
-      <c r="S1" s="148"/>
-      <c r="T1" s="148"/>
-      <c r="U1" s="148"/>
-      <c r="V1" s="148"/>
-      <c r="W1" s="148"/>
-      <c r="X1" s="148"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
+      <c r="M1" s="149"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="149"/>
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
+      <c r="U1" s="149"/>
+      <c r="V1" s="149"/>
+      <c r="W1" s="149"/>
+      <c r="X1" s="149"/>
     </row>
     <row r="2" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
-      <c r="U2" s="148"/>
-      <c r="V2" s="148"/>
-      <c r="W2" s="148"/>
-      <c r="X2" s="148"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
+      <c r="O2" s="149"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="149"/>
+      <c r="U2" s="149"/>
+      <c r="V2" s="149"/>
+      <c r="W2" s="149"/>
+      <c r="X2" s="149"/>
     </row>
     <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="156"/>
       <c r="D3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="155" t="s">
+      <c r="E3" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
-      <c r="K3" s="155"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="155"/>
-      <c r="O3" s="155"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="155"/>
-      <c r="R3" s="155"/>
-      <c r="S3" s="155"/>
-      <c r="T3" s="155"/>
-      <c r="U3" s="155"/>
-      <c r="V3" s="155"/>
-      <c r="W3" s="155"/>
-      <c r="X3" s="155"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="151"/>
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="151"/>
+      <c r="R3" s="151"/>
+      <c r="S3" s="151"/>
+      <c r="T3" s="151"/>
+      <c r="U3" s="151"/>
+      <c r="V3" s="151"/>
+      <c r="W3" s="151"/>
+      <c r="X3" s="151"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
         <v>1</v>
       </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
       <c r="D4" s="50"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="148"/>
-      <c r="S4" s="148"/>
-      <c r="T4" s="148"/>
-      <c r="U4" s="148"/>
-      <c r="V4" s="148"/>
-      <c r="W4" s="148"/>
-      <c r="X4" s="148"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="149"/>
+      <c r="G4" s="149"/>
+      <c r="H4" s="149"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="149"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="149"/>
+      <c r="N4" s="149"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="149"/>
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="149"/>
+      <c r="V4" s="149"/>
+      <c r="W4" s="149"/>
+      <c r="X4" s="149"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>2</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="153"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="152"/>
       <c r="D5" s="25"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="148"/>
-      <c r="K5" s="148"/>
-      <c r="L5" s="148"/>
-      <c r="M5" s="148"/>
-      <c r="N5" s="148"/>
-      <c r="O5" s="148"/>
-      <c r="P5" s="148"/>
-      <c r="Q5" s="148"/>
-      <c r="R5" s="148"/>
-      <c r="S5" s="148"/>
-      <c r="T5" s="148"/>
-      <c r="U5" s="148"/>
-      <c r="V5" s="148"/>
-      <c r="W5" s="148"/>
-      <c r="X5" s="148"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
+      <c r="M5" s="149"/>
+      <c r="N5" s="149"/>
+      <c r="O5" s="149"/>
+      <c r="P5" s="149"/>
+      <c r="Q5" s="149"/>
+      <c r="R5" s="149"/>
+      <c r="S5" s="149"/>
+      <c r="T5" s="149"/>
+      <c r="U5" s="149"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
+      <c r="X5" s="149"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>3</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="149"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="153"/>
-      <c r="M6" s="153"/>
-      <c r="N6" s="153"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="153"/>
-      <c r="Q6" s="153"/>
-      <c r="R6" s="153"/>
-      <c r="S6" s="153"/>
-      <c r="T6" s="153"/>
-      <c r="U6" s="153"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="153"/>
-      <c r="X6" s="153"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
+      <c r="H6" s="152"/>
+      <c r="I6" s="152"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="152"/>
+      <c r="M6" s="152"/>
+      <c r="N6" s="152"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
+      <c r="R6" s="152"/>
+      <c r="S6" s="152"/>
+      <c r="T6" s="152"/>
+      <c r="U6" s="152"/>
+      <c r="V6" s="152"/>
+      <c r="W6" s="152"/>
+      <c r="X6" s="152"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>4</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="148"/>
+      <c r="B7" s="149"/>
+      <c r="C7" s="149"/>
       <c r="D7" s="50"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="153"/>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
-      <c r="T7" s="153"/>
-      <c r="U7" s="153"/>
-      <c r="V7" s="153"/>
-      <c r="W7" s="153"/>
-      <c r="X7" s="153"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="152"/>
+      <c r="J7" s="152"/>
+      <c r="K7" s="152"/>
+      <c r="L7" s="152"/>
+      <c r="M7" s="152"/>
+      <c r="N7" s="152"/>
+      <c r="O7" s="152"/>
+      <c r="P7" s="152"/>
+      <c r="Q7" s="152"/>
+      <c r="R7" s="152"/>
+      <c r="S7" s="152"/>
+      <c r="T7" s="152"/>
+      <c r="U7" s="152"/>
+      <c r="V7" s="152"/>
+      <c r="W7" s="152"/>
+      <c r="X7" s="152"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>5</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="148"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="149"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="153"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153"/>
-      <c r="I8" s="153"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="153"/>
-      <c r="O8" s="153"/>
-      <c r="P8" s="153"/>
-      <c r="Q8" s="153"/>
-      <c r="R8" s="153"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="153"/>
-      <c r="U8" s="153"/>
-      <c r="V8" s="153"/>
-      <c r="W8" s="153"/>
-      <c r="X8" s="153"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="152"/>
+      <c r="K8" s="152"/>
+      <c r="L8" s="152"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="152"/>
+      <c r="O8" s="152"/>
+      <c r="P8" s="152"/>
+      <c r="Q8" s="152"/>
+      <c r="R8" s="152"/>
+      <c r="S8" s="152"/>
+      <c r="T8" s="152"/>
+      <c r="U8" s="152"/>
+      <c r="V8" s="152"/>
+      <c r="W8" s="152"/>
+      <c r="X8" s="152"/>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>6</v>
       </c>
-      <c r="B9" s="148"/>
-      <c r="C9" s="148"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="149"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="148"/>
-      <c r="T9" s="148"/>
-      <c r="U9" s="148"/>
-      <c r="V9" s="148"/>
-      <c r="W9" s="148"/>
-      <c r="X9" s="148"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="149"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="149"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="149"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="149"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="149"/>
+      <c r="T9" s="149"/>
+      <c r="U9" s="149"/>
+      <c r="V9" s="149"/>
+      <c r="W9" s="149"/>
+      <c r="X9" s="149"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>7</v>
       </c>
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
+      <c r="B10" s="149"/>
+      <c r="C10" s="149"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="148"/>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="148"/>
-      <c r="P10" s="148"/>
-      <c r="Q10" s="148"/>
-      <c r="R10" s="148"/>
-      <c r="S10" s="148"/>
-      <c r="T10" s="148"/>
-      <c r="U10" s="148"/>
-      <c r="V10" s="148"/>
-      <c r="W10" s="148"/>
-      <c r="X10" s="148"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="149"/>
+      <c r="N10" s="149"/>
+      <c r="O10" s="149"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="149"/>
+      <c r="T10" s="149"/>
+      <c r="U10" s="149"/>
+      <c r="V10" s="149"/>
+      <c r="W10" s="149"/>
+      <c r="X10" s="149"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>8</v>
       </c>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="149"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="148"/>
-      <c r="I11" s="148"/>
-      <c r="J11" s="148"/>
-      <c r="K11" s="148"/>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
-      <c r="N11" s="148"/>
-      <c r="O11" s="148"/>
-      <c r="P11" s="148"/>
-      <c r="Q11" s="148"/>
-      <c r="R11" s="148"/>
-      <c r="S11" s="148"/>
-      <c r="T11" s="148"/>
-      <c r="U11" s="148"/>
-      <c r="V11" s="148"/>
-      <c r="W11" s="148"/>
-      <c r="X11" s="148"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="149"/>
+      <c r="K11" s="149"/>
+      <c r="L11" s="149"/>
+      <c r="M11" s="149"/>
+      <c r="N11" s="149"/>
+      <c r="O11" s="149"/>
+      <c r="P11" s="149"/>
+      <c r="Q11" s="149"/>
+      <c r="R11" s="149"/>
+      <c r="S11" s="149"/>
+      <c r="T11" s="149"/>
+      <c r="U11" s="149"/>
+      <c r="V11" s="149"/>
+      <c r="W11" s="149"/>
+      <c r="X11" s="149"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>9</v>
       </c>
-      <c r="B12" s="148"/>
-      <c r="C12" s="148"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="148"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="148"/>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
-      <c r="X12" s="148"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="149"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="149"/>
+      <c r="L12" s="149"/>
+      <c r="M12" s="149"/>
+      <c r="N12" s="149"/>
+      <c r="O12" s="149"/>
+      <c r="P12" s="149"/>
+      <c r="Q12" s="149"/>
+      <c r="R12" s="149"/>
+      <c r="S12" s="149"/>
+      <c r="T12" s="149"/>
+      <c r="U12" s="149"/>
+      <c r="V12" s="149"/>
+      <c r="W12" s="149"/>
+      <c r="X12" s="149"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>10</v>
       </c>
-      <c r="B13" s="148"/>
-      <c r="C13" s="148"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="149"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="148"/>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="148"/>
-      <c r="U13" s="148"/>
-      <c r="V13" s="148"/>
-      <c r="W13" s="148"/>
-      <c r="X13" s="148"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="149"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149"/>
+      <c r="M13" s="149"/>
+      <c r="N13" s="149"/>
+      <c r="O13" s="149"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="149"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="149"/>
+      <c r="U13" s="149"/>
+      <c r="V13" s="149"/>
+      <c r="W13" s="149"/>
+      <c r="X13" s="149"/>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25"/>
-      <c r="B14" s="156">
+      <c r="B14" s="150">
         <f>SUM(B4:C13)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="156"/>
+      <c r="C14" s="150"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="155" t="s">
+      <c r="E14" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="155"/>
+      <c r="F14" s="151"/>
       <c r="G14" s="49">
         <f>B14-J17</f>
         <v>0</v>
       </c>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="148"/>
-      <c r="O14" s="148"/>
-      <c r="P14" s="148"/>
-      <c r="Q14" s="148"/>
-      <c r="R14" s="148"/>
-      <c r="S14" s="148"/>
-      <c r="T14" s="148"/>
-      <c r="U14" s="148"/>
-      <c r="V14" s="148"/>
-      <c r="W14" s="148"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="149"/>
+      <c r="L14" s="149"/>
+      <c r="M14" s="149"/>
+      <c r="N14" s="149"/>
+      <c r="O14" s="149"/>
+      <c r="P14" s="149"/>
+      <c r="Q14" s="149"/>
+      <c r="R14" s="149"/>
+      <c r="S14" s="149"/>
+      <c r="T14" s="149"/>
+      <c r="U14" s="149"/>
+      <c r="V14" s="149"/>
+      <c r="W14" s="149"/>
       <c r="X14" s="25"/>
     </row>
     <row r="15" spans="1:24" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="149" t="s">
+      <c r="A15" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="149"/>
-      <c r="F15" s="149"/>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="150"/>
-      <c r="L15" s="150"/>
-      <c r="M15" s="150"/>
-      <c r="N15" s="150"/>
-      <c r="O15" s="150"/>
-      <c r="P15" s="150"/>
-      <c r="Q15" s="150"/>
-      <c r="R15" s="150"/>
-      <c r="S15" s="150"/>
-      <c r="T15" s="150"/>
-      <c r="U15" s="150"/>
-      <c r="V15" s="150"/>
-      <c r="W15" s="150"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="148"/>
+      <c r="I15" s="148"/>
+      <c r="J15" s="148"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="148"/>
+      <c r="N15" s="148"/>
+      <c r="O15" s="148"/>
+      <c r="P15" s="148"/>
+      <c r="Q15" s="148"/>
+      <c r="R15" s="148"/>
+      <c r="S15" s="148"/>
+      <c r="T15" s="148"/>
+      <c r="U15" s="148"/>
+      <c r="V15" s="148"/>
+      <c r="W15" s="148"/>
       <c r="X15" s="25"/>
     </row>
     <row r="16" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -33046,6 +33052,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:X2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:X3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:X9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:X10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:X11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:X12"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="G15:W15"/>
     <mergeCell ref="B13:C13"/>
@@ -33053,30 +33083,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="H14:W14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:X10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:X11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:X12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:X9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:X6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:X1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:X2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>